<commit_message>
Add support for XLSX to spec-typed columns
</commit_message>
<xml_diff>
--- a/_test/test.xlsx
+++ b/_test/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="0" windowWidth="27825" windowHeight="12885"/>
+    <workbookView xWindow="2925" yWindow="0" windowWidth="27825" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="S1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>color</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>#000</t>
+  </si>
+  <si>
+    <t>optimized</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>count</t>
   </si>
 </sst>
 </file>
@@ -422,7 +434,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,68 +443,116 @@
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="10:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix panic on null cells
</commit_message>
<xml_diff>
--- a/_test/test.xlsx
+++ b/_test/test.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>color</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>#aaa</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>#fff</t>
   </si>
 </sst>
 </file>
@@ -434,7 +446,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,6 +567,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
     <row r="24" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J24" s="2"/>
     </row>

</xml_diff>